<commit_message>
updated status in req
</commit_message>
<xml_diff>
--- a/input-data-1.xlsx
+++ b/input-data-1.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://redbrickza-my.sharepoint.com/personal/ezekiel_mokaedi_rbconsult_co_za/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://redbrickza-my.sharepoint.com/personal/sipho_mancam_rbconsult_co_za/Documents/Documents/Programming/novapower/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1089" documentId="8_{46FBF132-2A8A-4D91-B50E-6F7DC39954D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4752887-E5D9-4AC9-99D5-E733C4E039C5}"/>
+  <xr:revisionPtr revIDLastSave="1104" documentId="8_{46FBF132-2A8A-4D91-B50E-6F7DC39954D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC3DA440-39A9-4776-84F8-0D4D34FAC878}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{A38C0819-823B-4194-AA2B-5033FF66305C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A38C0819-823B-4194-AA2B-5033FF66305C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$72</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="163">
   <si>
     <t>ItemName</t>
   </si>
@@ -503,6 +505,27 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Img Url</t>
+  </si>
+  <si>
+    <t>https://www.makro.co.za/sys-master/images/h06/h98/9800090222622/silo-MIN_237823_EAA_large</t>
+  </si>
+  <si>
+    <t>https://www.builders.co.za/_ui/responsive/theme-yellow/images/products/product-image-transparent.png</t>
+  </si>
+  <si>
+    <t>https://www.makro.co.za/sys-master/images/hc0/h4f/9800097300510/silo-MIN_159320_EAA_large</t>
+  </si>
+  <si>
+    <t>https://www.makro.co.za/sys-master/images/hba/h86/9800090746910/silo-MIN_285367_EAA_large</t>
+  </si>
+  <si>
+    <t>https://3pmedia.leroymerlin.co.za/SOURCE/a424840859ea40f38d972c635c8539ec</t>
+  </si>
+  <si>
+    <t>https://3pmedia.leroymerlin.co.za/SOURCE/10f337c37a7845719d921542d1415339</t>
   </si>
 </sst>
 </file>
@@ -512,7 +535,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-[$R-1C09]* #,##0_-;\-[$R-1C09]* #,##0_-;_-[$R-1C09]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -953,24 +976,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01BCF050-2F09-42D0-9049-6BF8B00124F4}">
-  <dimension ref="A1:G72"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H73" sqref="H73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="206.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="79.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.21875" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="79.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="91.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="15" thickBot="1">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -992,8 +1017,11 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1">
+      <c r="H1" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1017,7 +1045,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1">
+    <row r="3" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1041,7 +1069,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1">
+    <row r="4" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1065,7 +1093,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1">
+    <row r="5" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1089,7 +1117,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1">
+    <row r="6" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1113,7 +1141,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1">
+    <row r="7" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1137,7 +1165,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1">
+    <row r="8" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1161,7 +1189,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1">
+    <row r="9" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1185,7 +1213,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1">
+    <row r="10" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1209,7 +1237,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1">
+    <row r="11" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1233,7 +1261,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" thickBot="1">
+    <row r="12" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1257,7 +1285,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1">
+    <row r="13" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -1281,7 +1309,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1">
+    <row r="14" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -1305,7 +1333,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1">
+    <row r="15" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1329,7 +1357,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" thickBot="1">
+    <row r="16" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -1353,7 +1381,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" thickBot="1">
+    <row r="17" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -1377,7 +1405,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" thickBot="1">
+    <row r="18" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1401,7 +1429,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" thickBot="1">
+    <row r="19" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -1425,7 +1453,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1">
+    <row r="20" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -1449,7 +1477,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" thickBot="1">
+    <row r="21" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -1473,7 +1501,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15" thickBot="1">
+    <row r="22" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>58</v>
       </c>
@@ -1497,7 +1525,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15" thickBot="1">
+    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -1520,8 +1548,11 @@
       <c r="G23" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="15" thickBot="1">
+      <c r="H23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -1544,8 +1575,11 @@
       <c r="G24" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="15" thickBot="1">
+      <c r="H24" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>64</v>
       </c>
@@ -1568,8 +1602,11 @@
       <c r="G25" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="15" thickBot="1">
+      <c r="H25" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>64</v>
       </c>
@@ -1592,8 +1629,11 @@
       <c r="G26" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="15" thickBot="1">
+      <c r="H26" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -1616,8 +1656,11 @@
       <c r="G27" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="15">
+      <c r="H27" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>64</v>
       </c>
@@ -1639,8 +1682,11 @@
       <c r="G28" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="15">
+      <c r="H28" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -1662,8 +1708,11 @@
       <c r="G29" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="15" thickBot="1">
+      <c r="H29" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -1686,8 +1735,11 @@
       <c r="G30" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="15" thickBot="1">
+      <c r="H30" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>64</v>
       </c>
@@ -1710,8 +1762,11 @@
       <c r="G31" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" s="7" customFormat="1" ht="15" thickBot="1">
+      <c r="H31" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="7" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>13</v>
       </c>
@@ -1735,7 +1790,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15" thickBot="1">
+    <row r="33" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>13</v>
       </c>
@@ -1759,7 +1814,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15" thickBot="1">
+    <row r="34" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>13</v>
       </c>
@@ -1783,7 +1838,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15" thickBot="1">
+    <row r="35" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>18</v>
       </c>
@@ -1807,7 +1862,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15" thickBot="1">
+    <row r="36" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
         <v>18</v>
       </c>
@@ -1831,7 +1886,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15" thickBot="1">
+    <row r="37" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>18</v>
       </c>
@@ -1854,7 +1909,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15" thickBot="1">
+    <row r="38" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>18</v>
       </c>
@@ -1878,7 +1933,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15" thickBot="1">
+    <row r="39" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="8" t="s">
         <v>13</v>
       </c>
@@ -1902,7 +1957,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15" thickBot="1">
+    <row r="40" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="8" t="s">
         <v>13</v>
       </c>
@@ -1926,7 +1981,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15" thickBot="1">
+    <row r="41" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="8" t="s">
         <v>13</v>
       </c>
@@ -1950,7 +2005,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="15" thickBot="1">
+    <row r="42" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="8" t="s">
         <v>13</v>
       </c>
@@ -1974,7 +2029,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="15" thickBot="1">
+    <row r="43" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="8" t="s">
         <v>13</v>
       </c>
@@ -1998,7 +2053,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="15" thickBot="1">
+    <row r="44" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="8" t="s">
         <v>13</v>
       </c>
@@ -2022,7 +2077,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15" thickBot="1">
+    <row r="45" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="10" t="s">
         <v>13</v>
       </c>
@@ -2046,7 +2101,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="15" thickBot="1">
+    <row r="46" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="10" t="s">
         <v>13</v>
       </c>
@@ -2070,7 +2125,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="15" thickBot="1">
+    <row r="47" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="10" t="s">
         <v>13</v>
       </c>
@@ -2094,7 +2149,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="15" thickBot="1">
+    <row r="48" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="10" t="s">
         <v>13</v>
       </c>
@@ -2118,7 +2173,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="15" thickBot="1">
+    <row r="49" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="10" t="s">
         <v>13</v>
       </c>
@@ -2142,7 +2197,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="15" thickBot="1">
+    <row r="50" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="10" t="s">
         <v>18</v>
       </c>
@@ -2166,7 +2221,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="15" thickBot="1">
+    <row r="51" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="10" t="s">
         <v>18</v>
       </c>
@@ -2190,7 +2245,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="15" thickBot="1">
+    <row r="52" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="10" t="s">
         <v>18</v>
       </c>
@@ -2214,7 +2269,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="15" thickBot="1">
+    <row r="53" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="10" t="s">
         <v>13</v>
       </c>
@@ -2238,7 +2293,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="15" thickBot="1">
+    <row r="54" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="10" t="s">
         <v>13</v>
       </c>
@@ -2262,7 +2317,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="15" thickBot="1">
+    <row r="55" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="10" t="s">
         <v>13</v>
       </c>
@@ -2286,7 +2341,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="15" thickBot="1">
+    <row r="56" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="10" t="s">
         <v>13</v>
       </c>
@@ -2310,7 +2365,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="7" customFormat="1" ht="15" thickBot="1">
+    <row r="57" spans="1:7" s="7" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="12" t="s">
         <v>13</v>
       </c>
@@ -2334,7 +2389,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="58" spans="1:7" s="7" customFormat="1" ht="15" thickBot="1">
+    <row r="58" spans="1:7" s="7" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="12" t="s">
         <v>13</v>
       </c>
@@ -2358,7 +2413,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="59" spans="1:7" s="7" customFormat="1" ht="15" thickBot="1">
+    <row r="59" spans="1:7" s="7" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="12" t="s">
         <v>13</v>
       </c>
@@ -2382,7 +2437,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="60" spans="1:7" s="7" customFormat="1" ht="15" thickBot="1">
+    <row r="60" spans="1:7" s="7" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="12" t="s">
         <v>13</v>
       </c>
@@ -2406,7 +2461,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="61" spans="1:7" s="7" customFormat="1" ht="15" thickBot="1">
+    <row r="61" spans="1:7" s="7" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="12" t="s">
         <v>13</v>
       </c>
@@ -2430,7 +2485,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="62" spans="1:7" s="7" customFormat="1" ht="15" thickBot="1">
+    <row r="62" spans="1:7" s="7" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="12" t="s">
         <v>13</v>
       </c>
@@ -2454,7 +2509,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="63" spans="1:7" s="7" customFormat="1" ht="15" thickBot="1">
+    <row r="63" spans="1:7" s="7" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="12" t="s">
         <v>13</v>
       </c>
@@ -2478,7 +2533,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="64" spans="1:7" s="7" customFormat="1" ht="15" thickBot="1">
+    <row r="64" spans="1:7" s="7" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="12" t="s">
         <v>13</v>
       </c>
@@ -2502,7 +2557,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="15" thickBot="1">
+    <row r="65" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="12" t="s">
         <v>38</v>
       </c>
@@ -2526,7 +2581,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="15" thickBot="1">
+    <row r="66" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="12" t="s">
         <v>38</v>
       </c>
@@ -2550,7 +2605,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="15" thickBot="1">
+    <row r="67" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="12" t="s">
         <v>38</v>
       </c>
@@ -2574,7 +2629,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="15" thickBot="1">
+    <row r="68" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="13" t="s">
         <v>13</v>
       </c>
@@ -2598,7 +2653,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="15" thickBot="1">
+    <row r="69" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="13" t="s">
         <v>13</v>
       </c>
@@ -2622,7 +2677,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="15" thickBot="1">
+    <row r="70" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="13" t="s">
         <v>13</v>
       </c>
@@ -2646,7 +2701,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="15" thickBot="1">
+    <row r="71" spans="1:7" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="13" t="s">
         <v>13</v>
       </c>
@@ -2670,12 +2725,19 @@
         <v>127</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="C72" t="s">
         <v>155</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G72" xr:uid="{01BCF050-2F09-42D0-9049-6BF8B00124F4}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Generator"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" display="https://www.egadgets.co.za/mecer-3kva-3kw-solar-inverter-24v-1500mppt/" xr:uid="{3ECE821C-D2F9-4E95-9DD7-ADF947564077}"/>
@@ -2742,9 +2804,269 @@
     <hyperlink ref="F25" r:id="rId62" display="https://www.makro.co.za/hardware-auto/workshop-machinery/generators/generators/ryobi-5-5-kva-4-stroke-key-start-petrol-generator-/p/000000000000159320_EA" xr:uid="{EAEA13FC-A46F-4972-8AFE-8F83E73119BA}"/>
     <hyperlink ref="F23" r:id="rId63" display="https://www.makro.co.za/hardware-auto/workshop-machinery/generators/generators/ryobi-1-2-kva-pull-start-petrol-generator-/p/000000000000237823_EA" xr:uid="{FDD6C2F5-4A7E-45BD-9B76-695EA7C61655}"/>
     <hyperlink ref="F24" r:id="rId64" display="https://www.builders.co.za/Tools-%26-Protective-Wear/Power-Tools/Machinery/Generators/Ryobi-3-5kVA-4-Stoke-Petrol-Generator/p/000000000000641833?gclid=CjwKCAjwnZaVBhA6EiwAVVyv9KWWeUIqt8EZ6wE946feseNEMWKC2Rr4YRZJhpRtZv_J_teD-hiHGxoCfQMQAvD_BwE" xr:uid="{28892D4B-A93F-46E3-8D4C-7E3AFAF14301}"/>
-    <hyperlink ref="F28" r:id="rId65" xr:uid="{8212EFEC-AB53-41DB-8849-0156F734BD62}"/>
-    <hyperlink ref="F29" r:id="rId66" xr:uid="{597B458F-AC9A-476E-A0C1-37B53B57AA44}"/>
+    <hyperlink ref="F28" r:id="rId65" display="https://leroymerlin.co.za/3kva-key-start-diesel-generator?sfdr_ptcid=32806_617_672245882&amp;sfdr_hash=915149ff5b45d8e417fe7e3a2cab0093&amp;gclid=Cj0KCQjwwJuVBhCAARIsAOPwGAQbLkBUHN__lGFmbAd_LeIjYBn-W1p19Xt5i47UxVldhz3eHE9_QrcaAlP3EALw_wcB" xr:uid="{8212EFEC-AB53-41DB-8849-0156F734BD62}"/>
+    <hyperlink ref="F29" r:id="rId66" display="https://leroymerlin.co.za/7kva-key-start-diesel-generator?refSrc=77179&amp;nosto=nosto-page-product2" xr:uid="{597B458F-AC9A-476E-A0C1-37B53B57AA44}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100583804D756D08E4CA3423200232226B2" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b3af61a159263512a7f1ce494a3d6b52">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="38594f89-c314-49a7-8895-5d17cbb3f834" xmlns:ns3="c062e488-6187-499b-9180-094274b6916e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e65e6323747ef5a712f1b4f0f665253a" ns2:_="" ns3:_="">
+    <xsd:import namespace="38594f89-c314-49a7-8895-5d17cbb3f834"/>
+    <xsd:import namespace="c062e488-6187-499b-9180-094274b6916e"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="38594f89-c314-49a7-8895-5d17cbb3f834" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="11" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="12" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="15" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="17" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="18" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="19" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="20" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="23" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="4d832810-0dcb-4a40-af6c-905fa87ffd5b" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="c062e488-6187-499b-9180-094274b6916e" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="13" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="14" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="21" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{e9a75cdd-04e9-46a5-8769-fbdc5e8277c8}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="c062e488-6187-499b-9180-094274b6916e">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66141F94-59C4-4469-8581-D0FE08C86C69}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97A4A0F1-1ADB-4D11-AB6C-D7CA1761BFCE}"/>
 </file>
</xml_diff>